<commit_message>
[FSF] FrozenSnowFox Tweaks 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/FrozenSnowFox/[FSF] FrozenSnowFox Tweaks - 2893432492/[FSF] FrozenSnowFox Tweaks - 2893432492.xlsx
+++ b/Data/FrozenSnowFox/[FSF] FrozenSnowFox Tweaks - 2893432492/[FSF] FrozenSnowFox Tweaks - 2893432492.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SteamLibrary\steamapps\common\RimWorld\Mods\MOD KOREAN TRANSLATE\1.4\[FSF] FrozenSnowFox Tweaks - 2893432492\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{458E134E-B1E8-49D5-946E-BD0C8A40EDEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3A812B-A144-45FE-A855-B43EA1D84105}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="90" yWindow="2340" windowWidth="28710" windowHeight="11715" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Translate Here" sheetId="3" r:id="rId1"/>
-    <sheet name="Copy and Paste this into txt" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId2"/>
+    <sheet name="Copy and Paste this into txt" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="1070">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2156" uniqueCount="1083">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -3306,6 +3307,47 @@
   </si>
   <si>
     <t>강하 습격대 전략의 선택 가중치가 두 배로 증가합니다.  또한 습격 포인트 스케일링을 제거하여 강하 습격이 일반 습격과 동일한 크기로 진행되도록 합니다.</t>
+  </si>
+  <si>
+    <t>FSFTweaksCoreTweaksTitle</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FSFTweaksLoveIsBlindTitle</t>
+  </si>
+  <si>
+    <t>FSFTweaksLoveIsBlindDesc</t>
+  </si>
+  <si>
+    <t>FSFTweaksVFEDesertersMoreContrabandItemsTitle</t>
+  </si>
+  <si>
+    <t>FSFTweaksVFEDesertersMoreContrabandItemsDesc</t>
+  </si>
+  <si>
+    <t>Removes the romance chance reduction from genes allowing pawns to fall in love with whoever they like.</t>
+  </si>
+  <si>
+    <t>유전자에서 연애 확률 감소 효과를 제거하여 폰이 좋아하는 사람과 사랑에 빠질 수 있도록 합니다.</t>
+  </si>
+  <si>
+    <t>Love Is Blind</t>
+  </si>
+  <si>
+    <t>사랑은 장님</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>More Contraband Items</t>
+  </si>
+  <si>
+    <t>더 많은 밀수품</t>
+  </si>
+  <si>
+    <t>Adds a range of new contraband items to be purchased from the deserter network.  The items themselves are all Spacer and Ultra tech items.</t>
+  </si>
+  <si>
+    <t>탈영병 네트워크에서 구매할 수 있는 다양한 신규 밀수품 아이템이 추가됩니다.  아이템 자체는 모두 스페이서 및 울트라 기술 아이템입니다.</t>
   </si>
 </sst>
 </file>
@@ -3676,10 +3718,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCC57A9A-A004-4ADD-BAC8-AE0CD94EF67E}">
-  <dimension ref="A1:F355"/>
+  <dimension ref="A1:F359"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C334" workbookViewId="0">
-      <selection activeCell="E358" sqref="E358"/>
+    <sheetView tabSelected="1" topLeftCell="B345" workbookViewId="0">
+      <selection activeCell="E355" sqref="E355"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -9522,7 +9564,7 @@
     </row>
     <row r="324" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A324" t="str">
-        <f t="shared" ref="A324:A351" si="6">_xlfn.TEXTJOIN("+",,B324,C324)</f>
+        <f t="shared" ref="A324:A355" si="6">_xlfn.TEXTJOIN("+",,B324,C324)</f>
         <v>Keyed+FSFTweaksLargerPasteStorageOnDesc</v>
       </c>
       <c r="B324" t="s">
@@ -10025,70 +10067,142 @@
       </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A352" t="s">
+      <c r="A352" t="str">
+        <f t="shared" si="6"/>
+        <v>Keyed+FSFTweaksLoveIsBlindTitle</v>
+      </c>
+      <c r="B352" t="s">
+        <v>590</v>
+      </c>
+      <c r="C352" s="4" t="s">
+        <v>1071</v>
+      </c>
+      <c r="D352" s="4" t="s">
+        <v>1077</v>
+      </c>
+      <c r="E352" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A353" t="str">
+        <f t="shared" si="6"/>
+        <v>Keyed+FSFTweaksLoveIsBlindDesc</v>
+      </c>
+      <c r="B353" t="s">
+        <v>590</v>
+      </c>
+      <c r="C353" s="4" t="s">
+        <v>1072</v>
+      </c>
+      <c r="D353" s="4" t="s">
+        <v>1075</v>
+      </c>
+      <c r="E353" t="s">
+        <v>1076</v>
+      </c>
+    </row>
+    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A354" t="str">
+        <f t="shared" si="6"/>
+        <v>Keyed+FSFTweaksVFEDesertersMoreContrabandItemsTitle</v>
+      </c>
+      <c r="B354" t="s">
+        <v>590</v>
+      </c>
+      <c r="C354" s="4" t="s">
+        <v>1073</v>
+      </c>
+      <c r="D354" s="4" t="s">
+        <v>1079</v>
+      </c>
+      <c r="E354" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A355" t="str">
+        <f t="shared" si="6"/>
+        <v>Keyed+FSFTweaksVFEDesertersMoreContrabandItemsDesc</v>
+      </c>
+      <c r="B355" t="s">
+        <v>590</v>
+      </c>
+      <c r="C355" s="4" t="s">
+        <v>1074</v>
+      </c>
+      <c r="D355" s="4" t="s">
+        <v>1081</v>
+      </c>
+      <c r="E355" t="s">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A356" t="s">
         <v>701</v>
       </c>
-      <c r="B352" t="s">
+      <c r="B356" t="s">
         <v>702</v>
       </c>
-      <c r="C352" t="s">
+      <c r="C356" t="s">
         <v>703</v>
       </c>
-      <c r="D352" t="s">
+      <c r="D356" t="s">
         <v>704</v>
       </c>
-      <c r="E352" t="s">
+      <c r="E356" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A353" t="s">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A357" t="s">
         <v>706</v>
       </c>
-      <c r="B353" t="s">
+      <c r="B357" t="s">
         <v>702</v>
       </c>
-      <c r="C353" t="s">
+      <c r="C357" t="s">
         <v>707</v>
       </c>
-      <c r="D353" t="s">
+      <c r="D357" t="s">
         <v>708</v>
       </c>
-      <c r="E353" t="s">
+      <c r="E357" t="s">
         <v>709</v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A354" t="s">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A358" t="s">
         <v>710</v>
       </c>
-      <c r="B354" t="s">
+      <c r="B358" t="s">
         <v>711</v>
       </c>
-      <c r="C354" t="s">
+      <c r="C358" t="s">
         <v>712</v>
       </c>
-      <c r="D354" t="s">
+      <c r="D358" t="s">
         <v>713</v>
       </c>
-      <c r="E354" t="s">
+      <c r="E358" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A355" t="s">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A359" t="s">
         <v>715</v>
       </c>
-      <c r="B355" t="s">
+      <c r="B359" t="s">
         <v>711</v>
       </c>
-      <c r="C355" t="s">
+      <c r="C359" t="s">
         <v>716</v>
       </c>
-      <c r="D355" t="s">
+      <c r="D359" t="s">
         <v>717</v>
       </c>
-      <c r="E355" t="s">
+      <c r="E359" t="s">
         <v>718</v>
       </c>
     </row>
@@ -10099,11 +10213,2859 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A0112FC-4054-4D06-A8F2-010862B72A7A}">
+  <dimension ref="A1:F354"/>
+  <sheetViews>
+    <sheetView topLeftCell="A343" workbookViewId="0">
+      <selection activeCell="F351" sqref="F351:F354"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="F41" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F43" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F44" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="F46" s="4" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="F54" s="4" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="F56" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="F57" s="4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F59" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F60" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="F61" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F63" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="F65" s="4" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="F68" s="4" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F69" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A71" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F71" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="F72" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F73" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A74" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F75" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A76" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F76" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A77" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A78" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F78" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A79" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F79" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A80" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F80" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A81" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A82" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A83" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F83" s="4" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A84" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="F84" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A85" s="4" t="s">
+        <v>602</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A86" s="4" t="s">
+        <v>604</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A88" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="F88" s="4" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A89" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="F89" s="4" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A90" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="F90" s="4" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A91" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="F91" s="4" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A92" s="4" t="s">
+        <v>616</v>
+      </c>
+      <c r="F92" s="4" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A93" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A94" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="F94" s="4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A95" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="F95" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A96" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F96" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" s="4" t="s">
+        <v>618</v>
+      </c>
+      <c r="F97" s="4" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98" s="4" t="s">
+        <v>620</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="F99" s="4" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100" s="4" t="s">
+        <v>624</v>
+      </c>
+      <c r="F100" s="4" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="F101" s="4" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102" s="4" t="s">
+        <v>628</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104" s="4" t="s">
+        <v>631</v>
+      </c>
+      <c r="F104" s="4" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105" s="4" t="s">
+        <v>633</v>
+      </c>
+      <c r="F105" s="4" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="F106" s="4" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110" s="4" t="s">
+        <v>634</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111" s="4" t="s">
+        <v>636</v>
+      </c>
+      <c r="F111" s="4" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="F112" s="4" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F114" s="4" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="F115" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="F116" s="4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="F117" s="4" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="F118" s="4" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="F119" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="F120" s="4" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="F121" s="4" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="F122" s="4" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="F123" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F124" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125" s="4" t="s">
+        <v>638</v>
+      </c>
+      <c r="F125" s="4" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="F126" s="4" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="F127" s="4" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128" s="4" t="s">
+        <v>215</v>
+      </c>
+      <c r="F128" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A129" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F129" s="4" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A130" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="F130" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A131" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="F131" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A132" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="F132" s="4" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A133" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="F133" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A134" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="F134" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A135" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="F135" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A136" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F136" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A137" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="F137" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A138" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="F138" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A139" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F139" s="4" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A140" s="4" t="s">
+        <v>642</v>
+      </c>
+      <c r="F140" s="4" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A141" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="F141" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A142" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="F142" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A143" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="F143" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="144" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A144" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="F144" s="4" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A145" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="F145" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A146" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="F146" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A147" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="F147" s="4" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A148" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F148" s="4" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A149" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="F149" s="4" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A150" s="4" t="s">
+        <v>644</v>
+      </c>
+      <c r="F150" s="4" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A151" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="F151" s="4" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="F152" s="4" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A153" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="F153" s="4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F154" s="4" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="F155" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A156" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="F156" s="4" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A157" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="F157" s="4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A158" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="F158" s="4" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="F159" s="4" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A160" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="F160" s="4" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A161" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="F161" s="4" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A162" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="F162" s="4" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A163" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="F163" s="4" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A164" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="F164" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A165" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="F165" s="4" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A166" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="F166" s="4" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A167" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="F167" s="4" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A168" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="F168" s="4" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A169" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="F169" s="4" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A170" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="F170" s="4" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A171" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="F171" s="4" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A172" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="F172" s="4" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="173" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A173" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F173" s="4" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="174" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A174" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F174" s="4" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="175" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A175" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="F175" s="4" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="176" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A176" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="F176" s="4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="177" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A177" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="F177" s="4" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="178" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A178" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="F178" s="4" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="179" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A179" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F179" s="4" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="180" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A180" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="F180" s="4" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="181" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A181" s="4" t="s">
+        <v>315</v>
+      </c>
+      <c r="F181" s="4" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="182" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A182" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="F182" s="4" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="183" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A183" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="F183" s="4" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="184" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A184" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="F184" s="4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="185" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A185" s="4" t="s">
+        <v>319</v>
+      </c>
+      <c r="F185" s="4" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="186" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A186" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="F186" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="187" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A187" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="F187" s="4" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="188" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A188" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="F188" s="4" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="189" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A189" s="4" t="s">
+        <v>327</v>
+      </c>
+      <c r="F189" s="4" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="190" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A190" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="F190" s="4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A191" s="4" t="s">
+        <v>331</v>
+      </c>
+      <c r="F191" s="4" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A192" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="F192" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A193" s="4" t="s">
+        <v>335</v>
+      </c>
+      <c r="F193" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A194" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="F194" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A195" s="4" t="s">
+        <v>339</v>
+      </c>
+      <c r="F195" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A196" s="4" t="s">
+        <v>341</v>
+      </c>
+      <c r="F196" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A197" s="4" t="s">
+        <v>343</v>
+      </c>
+      <c r="F197" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A198" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="F198" s="4" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A199" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="F199" s="4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A200" s="4" t="s">
+        <v>349</v>
+      </c>
+      <c r="F200" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="201" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A201" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="F201" s="4" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="202" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A202" s="4" t="s">
+        <v>353</v>
+      </c>
+      <c r="F202" s="4" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="203" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A203" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="F203" s="4" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="204" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A204" s="4" t="s">
+        <v>653</v>
+      </c>
+      <c r="F204" s="4" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="205" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A205" s="4" t="s">
+        <v>355</v>
+      </c>
+      <c r="F205" s="4" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="206" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A206" s="4" t="s">
+        <v>357</v>
+      </c>
+      <c r="F206" s="4" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="207" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A207" s="4" t="s">
+        <v>359</v>
+      </c>
+      <c r="F207" s="4" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="208" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A208" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="F208" s="4" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A209" s="4" t="s">
+        <v>363</v>
+      </c>
+      <c r="F209" s="4" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A210" s="4" t="s">
+        <v>365</v>
+      </c>
+      <c r="F210" s="4" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A211" s="4" t="s">
+        <v>367</v>
+      </c>
+      <c r="F211" s="4" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A212" s="4" t="s">
+        <v>369</v>
+      </c>
+      <c r="F212" s="4" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A213" s="4" t="s">
+        <v>371</v>
+      </c>
+      <c r="F213" s="4" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A214" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="F214" s="4" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A215" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="F215" s="4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A216" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="F216" s="4" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A217" s="4" t="s">
+        <v>379</v>
+      </c>
+      <c r="F217" s="4" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A218" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="F218" s="4" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A219" s="4" t="s">
+        <v>383</v>
+      </c>
+      <c r="F219" s="4" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A220" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="F220" s="4" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A221" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="F221" s="4" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A222" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="F222" s="4" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A223" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="F223" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A224" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="F224" s="4" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="225" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A225" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="F225" s="4" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A226" s="4" t="s">
+        <v>397</v>
+      </c>
+      <c r="F226" s="4" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A227" s="4" t="s">
+        <v>399</v>
+      </c>
+      <c r="F227" s="4" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A228" s="4" t="s">
+        <v>401</v>
+      </c>
+      <c r="F228" s="4" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A229" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="F229" s="4" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A230" s="4" t="s">
+        <v>405</v>
+      </c>
+      <c r="F230" s="4" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A231" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="F231" s="4" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A232" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="F232" s="4" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A233" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="F233" s="4" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A234" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="F234" s="4" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="235" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A235" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="F235" s="4" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="236" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A236" s="4" t="s">
+        <v>417</v>
+      </c>
+      <c r="F236" s="4" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="237" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A237" s="4" t="s">
+        <v>419</v>
+      </c>
+      <c r="F237" s="4" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="238" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A238" s="4" t="s">
+        <v>421</v>
+      </c>
+      <c r="F238" s="4" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="239" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A239" s="4" t="s">
+        <v>423</v>
+      </c>
+      <c r="F239" s="4" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="240" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A240" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="F240" s="4" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="241" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A241" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="F241" s="4" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="242" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A242" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="F242" s="4" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="243" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A243" s="4" t="s">
+        <v>431</v>
+      </c>
+      <c r="F243" s="4" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="244" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A244" s="4" t="s">
+        <v>433</v>
+      </c>
+      <c r="F244" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="245" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A245" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="F245" s="4" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="246" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A246" s="4" t="s">
+        <v>437</v>
+      </c>
+      <c r="F246" s="4" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="247" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A247" s="4" t="s">
+        <v>438</v>
+      </c>
+      <c r="F247" s="4" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="248" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A248" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="F248" s="4" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="249" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A249" s="4" t="s">
+        <v>441</v>
+      </c>
+      <c r="F249" s="4" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="250" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A250" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="F250" s="4" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="251" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A251" s="4" t="s">
+        <v>445</v>
+      </c>
+      <c r="F251" s="4" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="252" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A252" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="F252" s="4" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="253" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A253" s="4" t="s">
+        <v>449</v>
+      </c>
+      <c r="F253" s="4" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="254" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A254" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="F254" s="4" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="255" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A255" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="F255" s="4" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="256" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A256" s="4" t="s">
+        <v>455</v>
+      </c>
+      <c r="F256" s="4" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="257" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A257" s="4" t="s">
+        <v>457</v>
+      </c>
+      <c r="F257" s="4" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="258" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A258" s="4" t="s">
+        <v>459</v>
+      </c>
+      <c r="F258" s="4" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="259" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A259" s="4" t="s">
+        <v>461</v>
+      </c>
+      <c r="F259" s="4" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A260" s="4" t="s">
+        <v>463</v>
+      </c>
+      <c r="F260" s="4" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A261" s="4" t="s">
+        <v>465</v>
+      </c>
+      <c r="F261" s="4" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A262" s="4" t="s">
+        <v>467</v>
+      </c>
+      <c r="F262" s="4" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A263" s="4" t="s">
+        <v>469</v>
+      </c>
+      <c r="F263" s="4" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A264" s="4" t="s">
+        <v>471</v>
+      </c>
+      <c r="F264" s="4" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A265" s="4" t="s">
+        <v>473</v>
+      </c>
+      <c r="F265" s="4" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A266" s="4" t="s">
+        <v>475</v>
+      </c>
+      <c r="F266" s="4" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A267" s="4" t="s">
+        <v>477</v>
+      </c>
+      <c r="F267" s="4" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A268" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="F268" s="4" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A269" s="4" t="s">
+        <v>480</v>
+      </c>
+      <c r="F269" s="4" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A270" s="4" t="s">
+        <v>481</v>
+      </c>
+      <c r="F270" s="4" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="271" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A271" s="4" t="s">
+        <v>482</v>
+      </c>
+      <c r="F271" s="4" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="272" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A272" s="4" t="s">
+        <v>484</v>
+      </c>
+      <c r="F272" s="4" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="273" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A273" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="F273" s="4" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="274" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A274" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="F274" s="4" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="275" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A275" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="F275" s="4" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="276" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A276" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="F276" s="4" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="277" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A277" s="4" t="s">
+        <v>488</v>
+      </c>
+      <c r="F277" s="4" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="278" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A278" s="4" t="s">
+        <v>490</v>
+      </c>
+      <c r="F278" s="4" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="279" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A279" s="4" t="s">
+        <v>492</v>
+      </c>
+      <c r="F279" s="4" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="280" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A280" s="4" t="s">
+        <v>494</v>
+      </c>
+      <c r="F280" s="4" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="281" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A281" s="4" t="s">
+        <v>496</v>
+      </c>
+      <c r="F281" s="4" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="282" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A282" s="4" t="s">
+        <v>663</v>
+      </c>
+      <c r="F282" s="4" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="283" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A283" s="4" t="s">
+        <v>665</v>
+      </c>
+      <c r="F283" s="4" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="284" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A284" s="4" t="s">
+        <v>667</v>
+      </c>
+      <c r="F284" s="4" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="285" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A285" s="4" t="s">
+        <v>498</v>
+      </c>
+      <c r="F285" s="4" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="286" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A286" s="4" t="s">
+        <v>500</v>
+      </c>
+      <c r="F286" s="4" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="287" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A287" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="F287" s="4" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="288" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A288" s="4" t="s">
+        <v>504</v>
+      </c>
+      <c r="F288" s="4" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="289" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A289" s="4" t="s">
+        <v>506</v>
+      </c>
+      <c r="F289" s="4" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="290" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A290" s="4" t="s">
+        <v>508</v>
+      </c>
+      <c r="F290" s="4" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="291" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A291" s="4" t="s">
+        <v>510</v>
+      </c>
+      <c r="F291" s="4" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="292" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A292" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="F292" s="4" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="293" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A293" s="4" t="s">
+        <v>514</v>
+      </c>
+      <c r="F293" s="4" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="294" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A294" s="4" t="s">
+        <v>516</v>
+      </c>
+      <c r="F294" s="4" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="295" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A295" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="F295" s="4" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="296" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A296" s="4" t="s">
+        <v>520</v>
+      </c>
+      <c r="F296" s="4" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="297" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A297" s="4" t="s">
+        <v>522</v>
+      </c>
+      <c r="F297" s="4" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="298" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A298" s="4" t="s">
+        <v>524</v>
+      </c>
+      <c r="F298" s="4" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="299" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A299" s="4" t="s">
+        <v>526</v>
+      </c>
+      <c r="F299" s="4" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="300" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A300" s="4" t="s">
+        <v>528</v>
+      </c>
+      <c r="F300" s="4" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="301" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A301" s="4" t="s">
+        <v>530</v>
+      </c>
+      <c r="F301" s="4" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="302" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A302" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="F302" s="4" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="303" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A303" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="F303" s="4" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="304" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A304" s="4" t="s">
+        <v>673</v>
+      </c>
+      <c r="F304" s="4" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="305" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A305" s="4" t="s">
+        <v>675</v>
+      </c>
+      <c r="F305" s="4" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="306" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A306" s="4" t="s">
+        <v>677</v>
+      </c>
+      <c r="F306" s="4" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="307" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A307" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="F307" s="4" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="308" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A308" s="4" t="s">
+        <v>681</v>
+      </c>
+      <c r="F308" s="4" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="309" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A309" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="F309" s="4" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="310" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A310" s="4" t="s">
+        <v>685</v>
+      </c>
+      <c r="F310" s="4" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="311" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A311" s="4" t="s">
+        <v>687</v>
+      </c>
+      <c r="F311" s="4" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="312" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A312" s="4" t="s">
+        <v>531</v>
+      </c>
+      <c r="F312" s="4" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="313" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A313" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="F313" s="4" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="314" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A314" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="F314" s="4" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="315" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A315" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="F315" s="4" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="316" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A316" s="4" t="s">
+        <v>539</v>
+      </c>
+      <c r="F316" s="4" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="317" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A317" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="F317" s="4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="318" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A318" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="F318" s="4" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="319" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A319" s="4" t="s">
+        <v>545</v>
+      </c>
+      <c r="F319" s="4" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="320" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A320" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="F320" s="4" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="321" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A321" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="F321" s="4" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="322" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A322" s="4" t="s">
+        <v>551</v>
+      </c>
+      <c r="F322" s="4" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="323" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A323" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="F323" s="4" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="324" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A324" s="4" t="s">
+        <v>555</v>
+      </c>
+      <c r="F324" s="4" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="325" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A325" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="F325" s="4" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="326" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A326" s="4" t="s">
+        <v>559</v>
+      </c>
+      <c r="F326" s="4" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="327" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A327" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="F327" s="4" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="328" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A328" s="4" t="s">
+        <v>563</v>
+      </c>
+      <c r="F328" s="4" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="329" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A329" s="4" t="s">
+        <v>690</v>
+      </c>
+      <c r="F329" s="4" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="330" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A330" s="4" t="s">
+        <v>692</v>
+      </c>
+      <c r="F330" s="4" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="331" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A331" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="F331" s="4" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="332" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A332" s="4" t="s">
+        <v>565</v>
+      </c>
+      <c r="F332" s="4" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="333" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A333" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="F333" s="4" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="334" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A334" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="F334" s="4" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="335" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A335" s="4" t="s">
+        <v>696</v>
+      </c>
+      <c r="F335" s="4" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="336" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A336" s="4" t="s">
+        <v>698</v>
+      </c>
+      <c r="F336" s="4" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="337" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A337" s="4" t="s">
+        <v>698</v>
+      </c>
+      <c r="F337" s="4" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="338" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A338" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="F338" s="4" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="339" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A339" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="F339" s="4" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="340" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A340" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="F340" s="4" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="341" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A341" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="F341" s="4" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="342" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A342" s="4" t="s">
+        <v>577</v>
+      </c>
+      <c r="F342" s="4" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="343" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A343" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="F343" s="4" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="344" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A344" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="F344" s="4" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="345" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A345" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="F345" s="4" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="346" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A346" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="F346" s="4" t="s">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="347" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A347" s="4" t="s">
+        <v>587</v>
+      </c>
+      <c r="F347" s="4" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="348" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A348" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="F348" s="4" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="349" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A349" s="4" t="s">
+        <v>1064</v>
+      </c>
+      <c r="F349" s="4" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="350" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A350" s="4" t="s">
+        <v>1065</v>
+      </c>
+      <c r="F350" s="4" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="351" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A351" t="s">
+        <v>703</v>
+      </c>
+      <c r="F351" s="4" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="352" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A352" t="s">
+        <v>707</v>
+      </c>
+      <c r="F352" s="4" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="353" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A353" t="s">
+        <v>712</v>
+      </c>
+      <c r="F353" s="4" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="354" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A354" t="s">
+        <v>716</v>
+      </c>
+      <c r="F354" s="4" t="s">
+        <v>1074</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92DC3856-64E6-47A8-8050-4BFF07C50F4A}">
-  <dimension ref="A1:A357"/>
+  <dimension ref="A1:A361"/>
   <sheetViews>
     <sheetView topLeftCell="A334" workbookViewId="0">
-      <selection activeCell="A61" sqref="A61"/>
+      <selection activeCell="A338" sqref="A338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -10123,7 +13085,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="str" cm="1">
-        <f t="array" ref="A3:A357">_xlfn.VSTACK(_xlfn.BYROW(_xlfn.LAMBDA(_xlpm.x,_xlfn.HSTACK(_xlfn.BYROW(_xlfn.CHOOSECOLS(_xlpm.x,1),_xlfn.LAMBDA(_xlpm.a,_xlfn.CONCAT("&lt;",_xlpm.a,"&gt;"))),_xlfn.CHOOSECOLS(_xlpm.x,2),_xlfn.BYROW(_xlfn.CHOOSECOLS(_xlpm.x,1),_xlfn.LAMBDA(_xlpm.b,_xlfn.CONCAT("&lt;/",_xlpm.b,"&gt;")))))(_xlfn._xlws.FILTER(_xlfn.HSTACK('Translate Here'!C2:C1002,'Translate Here'!E2:E1002),'Translate Here'!C2:C1002&lt;&gt;0)),_xlfn.LAMBDA(_xlpm.j,_xlfn.TEXTJOIN(,,_xlpm.j))),"&lt;/LanguageData&gt;")</f>
+        <f t="array" ref="A3:A361">_xlfn.VSTACK(_xlfn.BYROW(_xlfn.LAMBDA(_xlpm.x,_xlfn.HSTACK(_xlfn.BYROW(_xlfn.CHOOSECOLS(_xlpm.x,1),_xlfn.LAMBDA(_xlpm.a,_xlfn.CONCAT("&lt;",_xlpm.a,"&gt;"))),_xlfn.CHOOSECOLS(_xlpm.x,2),_xlfn.BYROW(_xlfn.CHOOSECOLS(_xlpm.x,1),_xlfn.LAMBDA(_xlpm.b,_xlfn.CONCAT("&lt;/",_xlpm.b,"&gt;")))))(_xlfn._xlws.FILTER(_xlfn.HSTACK('Translate Here'!C2:C1006,'Translate Here'!E2:E1006),'Translate Here'!C2:C1006&lt;&gt;0)),_xlfn.LAMBDA(_xlpm.j,_xlfn.TEXTJOIN(,,_xlpm.j))),"&lt;/LanguageData&gt;")</f>
         <v>&lt;FSFTweaksModWarning&gt;변경된 설정을 적용하려면 게임을 다시 시작해야 합니다.&lt;/FSFTweaksModWarning&gt;</v>
       </c>
     </row>
@@ -11874,26 +14836,46 @@
     </row>
     <row r="353" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A353" t="str">
-        <v>&lt;FSFNormalCarpetFine.label&gt;무늬없는 멋진 양탄자 ({0})&lt;/FSFNormalCarpetFine.label&gt;</v>
+        <v>&lt;FSFTweaksLoveIsBlindTitle&gt;사랑은 장님&lt;/FSFTweaksLoveIsBlindTitle&gt;</v>
       </c>
     </row>
     <row r="354" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A354" t="str">
-        <v>&lt;FSFNormalCarpetFine.description&gt;단색 섬유로 만든 고급스러운 양탄자입니다. 보기에 좋지만 청소하기 어렵습니다.&lt;/FSFNormalCarpetFine.description&gt;</v>
+        <v>&lt;FSFTweaksLoveIsBlindDesc&gt;유전자에서 연애 확률 감소 효과를 제거하여 폰이 좋아하는 사람과 사랑에 빠질 수 있도록 합니다.&lt;/FSFTweaksLoveIsBlindDesc&gt;</v>
       </c>
     </row>
     <row r="355" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A355" t="str">
-        <v>&lt;FSFBiodomeSunlamp.label&gt;바이오돔 태양등&lt;/FSFBiodomeSunlamp.label&gt;</v>
+        <v>&lt;FSFTweaksVFEDesertersMoreContrabandItemsTitle&gt;더 많은 밀수품&lt;/FSFTweaksVFEDesertersMoreContrabandItemsTitle&gt;</v>
       </c>
     </row>
     <row r="356" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A356" t="str">
-        <v>&lt;FSFBiodomeSunlamp.description&gt;전원이 필요 없고 투명한 바이오돔 천장 역할을 하도록 설계된 태양등입니다. 채광창이나 투명한 지붕을 추가하는 모드에 대한 간단한 대안이 될 수 있습니다.&lt;/FSFBiodomeSunlamp.description&gt;</v>
+        <v>&lt;FSFTweaksVFEDesertersMoreContrabandItemsDesc&gt;탈영병 네트워크에서 구매할 수 있는 다양한 신규 밀수품 아이템이 추가됩니다.  아이템 자체는 모두 스페이서 및 울트라 기술 아이템입니다.&lt;/FSFTweaksVFEDesertersMoreContrabandItemsDesc&gt;</v>
       </c>
     </row>
     <row r="357" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A357" t="str">
+        <v>&lt;FSFNormalCarpetFine.label&gt;무늬없는 멋진 양탄자 ({0})&lt;/FSFNormalCarpetFine.label&gt;</v>
+      </c>
+    </row>
+    <row r="358" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A358" t="str">
+        <v>&lt;FSFNormalCarpetFine.description&gt;단색 섬유로 만든 고급스러운 양탄자입니다. 보기에 좋지만 청소하기 어렵습니다.&lt;/FSFNormalCarpetFine.description&gt;</v>
+      </c>
+    </row>
+    <row r="359" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A359" t="str">
+        <v>&lt;FSFBiodomeSunlamp.label&gt;바이오돔 태양등&lt;/FSFBiodomeSunlamp.label&gt;</v>
+      </c>
+    </row>
+    <row r="360" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A360" t="str">
+        <v>&lt;FSFBiodomeSunlamp.description&gt;전원이 필요 없고 투명한 바이오돔 천장 역할을 하도록 설계된 태양등입니다. 채광창이나 투명한 지붕을 추가하는 모드에 대한 간단한 대안이 될 수 있습니다.&lt;/FSFBiodomeSunlamp.description&gt;</v>
+      </c>
+    </row>
+    <row r="361" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A361" t="str">
         <v>&lt;/LanguageData&gt;</v>
       </c>
     </row>

</xml_diff>